<commit_message>
Fix upload file quiz, file assignment
</commit_message>
<xml_diff>
--- a/server/uploads/quizz.xlsx
+++ b/server/uploads/quizz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam4\KLTN\Project_ELearning_KLTN\server\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9B937F-AC23-4016-B978-29BBBBB215E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A66E5EE-9292-434E-AC1D-5F7872BEA258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="12780" windowWidth="19410" windowHeight="8205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="2865" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>question</t>
   </si>
@@ -66,16 +66,10 @@
     <t>B: SQL là một loại ngôn ngữ lập trình</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>during_time</t>
   </si>
   <si>
     <t>passpoint</t>
-  </si>
-  <si>
-    <t>Quizz ôn tập</t>
   </si>
   <si>
     <t>title</t>
@@ -413,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +422,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -436,10 +430,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,58 +441,50 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>